<commit_message>
wave csv passing complte
</commit_message>
<xml_diff>
--- a/Client/Resources/Data/ObjectArrange/ObjectArrange.xlsx
+++ b/Client/Resources/Data/ObjectArrange/ObjectArrange.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ArcheTypeZero\GA_6th_2Q_Project\Client\Resources\Data\ObjectArrange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8392700F-C539-4A34-9DB1-1B1E1A5F04F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15EF327-22BD-4457-A0C0-D19B59B5E5C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Stage1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Gridx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ObjectName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>player</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,15 +377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -383,13 +395,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -397,7 +412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -407,8 +422,11 @@
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -418,8 +436,11 @@
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -429,8 +450,11 @@
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -440,8 +464,11 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>99</v>
       </c>
@@ -451,8 +478,11 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -462,8 +492,11 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -473,8 +506,11 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -484,8 +520,11 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -495,8 +534,11 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -505,6 +547,9 @@
       </c>
       <c r="C13">
         <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fix & ToolTip mod
카드 선택창에서 툴팁 이상한 위치에 뜨던거 수정
</commit_message>
<xml_diff>
--- a/Client/Resources/Data/ObjectArrange/ObjectArrange.xlsx
+++ b/Client/Resources/Data/ObjectArrange/ObjectArrange.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ArcheTypeZero\GA_6th_2Q_Project\Client\Resources\Data\ObjectArrange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F8C5D0-FA34-4A9C-981E-6850C3F72BF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316626A8-8BDA-4826-A4B8-A627750DBFE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="16">
   <si>
     <t>ObjectID</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G66" activeCellId="1" sqref="A64:D78 G66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1237,7 +1237,7 @@
         <v>15</v>
       </c>
       <c r="B62">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,30 +1256,30 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B64">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1287,10 +1287,10 @@
         <v>5</v>
       </c>
       <c r="B66">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1298,30 +1298,30 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1329,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1343,10 +1343,10 @@
         <v>2</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -1357,10 +1357,10 @@
         <v>2</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -1371,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="B72">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1382,30 +1382,30 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C75">
         <v>6</v>
@@ -1427,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C76">
         <v>6</v>
@@ -1441,7 +1441,7 @@
         <v>3</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C77">
         <v>6</v>
@@ -1455,12 +1455,40 @@
         <v>3</v>
       </c>
       <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79">
         <v>15</v>
       </c>
-      <c r="C78">
-        <v>5</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>15</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>